<commit_message>
Updated the chart legend
</commit_message>
<xml_diff>
--- a/benchmark_results/hfc-bench-graph.xlsx
+++ b/benchmark_results/hfc-bench-graph.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4503E33C-3761-4910-B75D-E16ACB94B528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4E3E4D-C181-49DF-A57F-7F94F280E122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{2D049191-F8BF-44D6-9CF7-7569348EF50F}"/>
+    <workbookView xWindow="45972" yWindow="-216" windowWidth="46296" windowHeight="25416" xr2:uid="{2D049191-F8BF-44D6-9CF7-7569348EF50F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t>cmake + Hermetic FetchContent</t>
   </si>
   <si>
-    <t>cmake-re + Hermetic FetchContent</t>
-  </si>
-  <si>
     <t>AWS EC2 c7a.4xlarge</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>Per conf s</t>
+  </si>
+  <si>
+    <t>cmake-re L1 + Hermetic FetchContent</t>
   </si>
 </sst>
 </file>
@@ -340,7 +340,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>cmake-re + Hermetic FetchContent</c:v>
+                  <c:v>cmake-re L1 + Hermetic FetchContent</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -932,7 +932,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>cmake-re + Hermetic FetchContent</c:v>
+                  <c:v>cmake-re L1 + Hermetic FetchContent</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2888,8 +2888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3999E18-4547-4AB7-A730-B0419250327F}">
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X9" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="AK12" sqref="AK12"/>
+    <sheetView tabSelected="1" topLeftCell="V9" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="AB13" sqref="AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2904,7 +2904,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="72" x14ac:dyDescent="0.3">
@@ -2928,7 +2928,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>0</v>
@@ -2947,7 +2947,7 @@
         <v>12</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -3255,7 +3255,7 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="72" x14ac:dyDescent="0.3">
@@ -3279,7 +3279,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>0</v>
@@ -3298,7 +3298,7 @@
         <v>12</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
@@ -3522,7 +3522,7 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="5">
         <f>AVERAGE(B24:B28)/1000</f>
@@ -3569,7 +3569,7 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31">
         <f>B29/4</f>

</xml_diff>